<commit_message>
Complete the test class
</commit_message>
<xml_diff>
--- a/generatedFile/test.xlsx
+++ b/generatedFile/test.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="42">
   <si>
     <t>courseNo</t>
   </si>
@@ -134,7 +134,10 @@
     <t>11</t>
   </si>
   <si>
-    <t>Test</t>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>3.0</t>
   </si>
 </sst>
 </file>
@@ -416,10 +419,10 @@
         <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F12" t="s">
         <v>28</v>

</xml_diff>